<commit_message>
updated archived version of temoa to version 9d10c1d from June 30, 2020
This is the last version before introduction of regionalization

 Link to download:  https://github.com/TemoaProject/temoa/tree/9d10c1da81dc6b4f2b34cadfac9db947251254e2
</commit_message>
<xml_diff>
--- a/examples/baselines/data/data.xlsx
+++ b/examples/baselines/data/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03CFB8F-7531-4660-AED0-28542FE41559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05040B8-9548-4920-8F7E-F0F4D9E44748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -14,16 +14,18 @@
     <sheet name="Connections" sheetId="1" r:id="rId4"/>
     <sheet name="Demand" sheetId="3" r:id="rId5"/>
     <sheet name="ConnectionsExisting" sheetId="2" r:id="rId6"/>
-    <sheet name="DiscountRate" sheetId="5" r:id="rId7"/>
-    <sheet name="Fuels" sheetId="6" r:id="rId8"/>
-    <sheet name="FuelsExisting" sheetId="7" r:id="rId9"/>
-    <sheet name="PowerPlants" sheetId="8" r:id="rId10"/>
-    <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId11"/>
-    <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId12"/>
-    <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId13"/>
-    <sheet name="PowerPlantsExisting" sheetId="11" r:id="rId14"/>
-    <sheet name="ReserveMargin" sheetId="13" r:id="rId15"/>
-    <sheet name="capacityFactorTOD" sheetId="14" r:id="rId16"/>
+    <sheet name="DiscountRateGlobal" sheetId="5" r:id="rId7"/>
+    <sheet name="DiscountRateTech" sheetId="19" r:id="rId8"/>
+    <sheet name="Emission" sheetId="20" r:id="rId9"/>
+    <sheet name="Fuels" sheetId="6" r:id="rId10"/>
+    <sheet name="FuelsExisting" sheetId="7" r:id="rId11"/>
+    <sheet name="PowerPlants" sheetId="8" r:id="rId12"/>
+    <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId13"/>
+    <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId14"/>
+    <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId15"/>
+    <sheet name="PowerPlantsExisting" sheetId="11" r:id="rId16"/>
+    <sheet name="ReserveMargin" sheetId="13" r:id="rId17"/>
+    <sheet name="capacityFactorTOD" sheetId="14" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="235">
   <si>
     <t>connection</t>
   </si>
@@ -707,6 +709,45 @@
   </si>
   <si>
     <t>[fr]</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>vintage</t>
+  </si>
+  <si>
+    <t>tech_rate</t>
+  </si>
+  <si>
+    <t>tech_rate_notes</t>
+  </si>
+  <si>
+    <t>[name]</t>
+  </si>
+  <si>
+    <t>periods</t>
+  </si>
+  <si>
+    <t>emis_comm</t>
+  </si>
+  <si>
+    <t>emis_limit</t>
+  </si>
+  <si>
+    <t>emis_limit_units</t>
+  </si>
+  <si>
+    <t>emis_limit_notes</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>real</t>
   </si>
 </sst>
 </file>
@@ -1383,10 +1424,379 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3">
+        <v>5.7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3">
+        <v>2.66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4">
+        <v>4.03</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4">
+        <v>2.7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4">
+        <v>90.37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>11.46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5">
+        <v>2.8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5">
+        <v>69.34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>39.51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>7.19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8">
+        <v>3.05</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8">
+        <v>67.58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9">
+        <v>7.62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="1">
+        <v>63.3</v>
+      </c>
+      <c r="H9">
+        <v>50.3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1920</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3:I28"/>
     </sheetView>
   </sheetViews>
@@ -2147,7 +2557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -2866,7 +3276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -3497,7 +3907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3846,7 +4256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -4231,7 +4641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4272,7 +4682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
@@ -7005,7 +7415,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7044,367 +7454,90 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE35283-3BE3-4F5A-8433-3D888AE7F852}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>222</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>224</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>226</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>77</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3">
-        <v>5.7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3">
-        <v>2.66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3">
-        <v>40</v>
-      </c>
-      <c r="K3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4">
-        <v>4.03</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4">
-        <v>2.7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4">
-        <v>90.37</v>
-      </c>
-      <c r="I4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5">
-        <v>11.46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5">
-        <v>2.8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5">
-        <v>69.34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>40</v>
-      </c>
-      <c r="K6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>39.51</v>
-      </c>
-      <c r="I7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7">
-        <v>40</v>
-      </c>
-      <c r="K7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8">
-        <v>7.19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8">
-        <v>3.05</v>
-      </c>
-      <c r="E8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8">
-        <v>67.58</v>
-      </c>
-      <c r="I8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9">
-        <v>7.62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="E9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="1">
-        <v>63.3</v>
-      </c>
-      <c r="H9">
-        <v>50.3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9">
-        <v>40</v>
-      </c>
-      <c r="K9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>40</v>
-      </c>
-      <c r="K10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>40</v>
-      </c>
-      <c r="K11" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F44819-0382-4850-9146-7C529C159FEB}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="E13" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>233</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1920</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2015</v>
+        <v>233</v>
+      </c>
+      <c r="E2" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverted baselines_run.py to be the same as original temoatools repo
adding energy storage duration part 1
updated data.xlsx and db_schema_temoa_mod.sqlite to incorporate energy storage duration parameter
</commit_message>
<xml_diff>
--- a/examples/baselines/data/data.xlsx
+++ b/examples/baselines/data/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05040B8-9548-4920-8F7E-F0F4D9E44748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5D2E9A-4542-4967-B724-80B7F29F5E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -32,18 +32,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="237">
   <si>
     <t>connection</t>
   </si>
@@ -748,6 +742,12 @@
   </si>
   <si>
     <t>real</t>
+  </si>
+  <si>
+    <t>StorageDuration</t>
+  </si>
+  <si>
+    <t>[hr]</t>
   </si>
 </sst>
 </file>
@@ -1794,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,9 +1805,11 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1835,8 +1837,11 @@
       <c r="I1" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>70</v>
       </c>
@@ -1864,8 +1869,11 @@
       <c r="I2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -1891,7 +1899,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -1917,7 +1925,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -1943,7 +1951,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -1969,7 +1977,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -1995,7 +2003,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -2021,7 +2029,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -2047,7 +2055,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
@@ -2073,7 +2081,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -2099,7 +2107,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -2125,7 +2133,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -2151,7 +2159,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>117</v>
       </c>
@@ -2176,8 +2184,11 @@
       <c r="H14" s="22" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>118</v>
       </c>
@@ -2203,7 +2214,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>215</v>
       </c>
@@ -2229,7 +2240,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>216</v>
       </c>
@@ -2255,7 +2266,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>218</v>
       </c>
@@ -2281,7 +2292,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>119</v>
       </c>
@@ -2307,7 +2318,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>120</v>
       </c>
@@ -2333,7 +2344,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>121</v>
       </c>
@@ -2359,7 +2370,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>122</v>
       </c>
@@ -2385,7 +2396,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
@@ -2410,8 +2421,11 @@
       <c r="H23" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -2437,7 +2451,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -2463,7 +2477,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
@@ -2489,7 +2503,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -2515,7 +2529,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -7457,7 +7471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE35283-3BE3-4F5A-8433-3D888AE7F852}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding energy storage duration part 2 completed adding energy storage duration temoatools to match temoa implementation
updated example cases and virginia project to all include StorageDuration parameter which is set in hours. This parameter is now required for all storage technologies
</commit_message>
<xml_diff>
--- a/examples/baselines/data/data.xlsx
+++ b/examples/baselines/data/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5D2E9A-4542-4967-B724-80B7F29F5E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF0C7B-41C2-4E8A-98E2-B03DA98E5D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Emission" sheetId="20" r:id="rId9"/>
     <sheet name="Fuels" sheetId="6" r:id="rId10"/>
     <sheet name="FuelsExisting" sheetId="7" r:id="rId11"/>
-    <sheet name="PowerPlants" sheetId="8" r:id="rId12"/>
-    <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId13"/>
+    <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId12"/>
+    <sheet name="PowerPlants" sheetId="8" r:id="rId13"/>
     <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId14"/>
     <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId15"/>
     <sheet name="PowerPlantsExisting" sheetId="11" r:id="rId16"/>
@@ -1739,7 +1739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -1793,785 +1793,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="J23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D3:H15 D19:H28">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:H18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -3285,6 +2506,786 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:H15 D19:H28">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:H18">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 'About' sheet to data.xlsx to explain what it is and how variables are used
Added new entries to VA project (costs that change by year and introduction years for technologies)
</commit_message>
<xml_diff>
--- a/examples/baselines/data/data.xlsx
+++ b/examples/baselines/data/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6BDEF4-6481-43E6-A41F-7EC761A5C1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C546448-4D9A-4DE9-9080-9FE336276559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="M1" sqref="M1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2633,7 +2633,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4173,7 +4173,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H1" sqref="H1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5003,7 +5003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7059,7 +7059,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N1" sqref="N1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7683,7 +7683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -7816,7 +7816,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7902,25 +7902,25 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E12:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>230</v>
       </c>
     </row>

</xml_diff>